<commit_message>
finalisation de rest et orm
</commit_message>
<xml_diff>
--- a/Nouveau livre/Quizz.xlsx
+++ b/Nouveau livre/Quizz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kotlin be back\Kotlin_be_back\Nouveau livre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A509F32-000C-4C8C-97CD-F22E357A5F34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2496A3C-0EE3-4936-9597-D145BDCBAB7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="147">
   <si>
     <t>01 Présentation de l’environnement OK</t>
   </si>
@@ -54,15 +54,6 @@
     <t>09 ViewModel et LiveData OK</t>
   </si>
   <si>
-    <t>10 L’ORM Room</t>
-  </si>
-  <si>
-    <t>11 RecyclerView</t>
-  </si>
-  <si>
-    <t>12 Communiquer avec une API REST</t>
-  </si>
-  <si>
     <t>13 Firebase</t>
   </si>
   <si>
@@ -388,6 +379,93 @@
   </si>
   <si>
     <t>Firebase est 100% gratuit</t>
+  </si>
+  <si>
+    <t>Dans quel fichier sont listé les activités d'una application ?</t>
+  </si>
+  <si>
+    <t>Android Manifest.xml</t>
+  </si>
+  <si>
+    <t>Dans quel fichier sont listé les permissions necessaires à l'application ?</t>
+  </si>
+  <si>
+    <t>Une application peut elle ouvrir une autre application ?</t>
+  </si>
+  <si>
+    <t>Quelle balise permet de specifier le role d'une activité ?</t>
+  </si>
+  <si>
+    <t>&lt;intent-filter&gt;</t>
+  </si>
+  <si>
+    <t>Bonne Réponse</t>
+  </si>
+  <si>
+    <t>Fausse réponse</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Firebase</t>
+  </si>
+  <si>
+    <t>un téléphone Google</t>
+  </si>
+  <si>
+    <t>un Etui</t>
+  </si>
+  <si>
+    <t>un logiciel</t>
+  </si>
+  <si>
+    <t>Eclipse</t>
+  </si>
+  <si>
+    <t>Visual Studio Code</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Maven</t>
+  </si>
+  <si>
+    <t>npm</t>
+  </si>
+  <si>
+    <t>composer</t>
+  </si>
+  <si>
+    <t>LinearLayout</t>
+  </si>
+  <si>
+    <t>GridLayout</t>
+  </si>
+  <si>
+    <t>RelativeLayout</t>
+  </si>
+  <si>
+    <t>Json</t>
+  </si>
+  <si>
+    <t>Html</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>10 L’ORM Room OK</t>
+  </si>
+  <si>
+    <t>11 RecyclerView OK</t>
+  </si>
+  <si>
+    <t>12 Communiquer avec une API REST OK</t>
   </si>
 </sst>
 </file>
@@ -417,7 +495,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +505,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -458,6 +548,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,155 +832,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="91.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2">
         <v>2017</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2016</v>
+      </c>
+      <c r="D3">
+        <v>1970</v>
+      </c>
+      <c r="E3">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -896,33 +1067,33 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -932,23 +1103,23 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2" t="b">
         <v>1</v>
@@ -956,7 +1127,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="b">
         <v>0</v>
@@ -964,10 +1135,10 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -977,39 +1148,39 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="b">
         <v>1</v>
@@ -1022,23 +1193,43 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
@@ -1047,7 +1238,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B44" s="2" t="b">
         <v>1</v>
@@ -1055,37 +1246,37 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1095,84 +1286,84 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B60" s="2" t="b">
         <v>1</v>
@@ -1180,118 +1371,118 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>10</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B76" s="2" t="b">
         <v>1</v>
@@ -1299,7 +1490,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B77" s="2" t="b">
         <v>1</v>
@@ -1307,7 +1498,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B78" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
ajout de demos dans chapitre 5
</commit_message>
<xml_diff>
--- a/Nouveau livre/Quizz.xlsx
+++ b/Nouveau livre/Quizz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kotlin_be_back\Kotlin_be_back\Nouveau livre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C792B1-2EC9-44E6-A67F-84924980FC80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C10A0E4-AF05-4951-835B-A353EF58CC08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="150">
   <si>
     <t>01 Présentation de l’environnement OK</t>
   </si>
@@ -879,7 +879,7 @@
   <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +894,7 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8">
         <f>SUM(A2:A88)</f>
-        <v>147936</v>
+        <v>175381</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>147</v>
@@ -1209,10 +1209,19 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>27445</v>
+      </c>
+      <c r="B26">
+        <f>SUM(A2:A26)/5</f>
+        <v>35076.199999999997</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">

</xml_diff>

<commit_message>
fin des démo pour le chapitre9
</commit_message>
<xml_diff>
--- a/Nouveau livre/Quizz.xlsx
+++ b/Nouveau livre/Quizz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kotlin_be_back\Kotlin_be_back\Nouveau livre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C10A0E4-AF05-4951-835B-A353EF58CC08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B0C041-978E-4B6B-B0B3-BF1A8A653A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
   <si>
     <t>01 Présentation de l’environnement OK</t>
   </si>
@@ -50,9 +50,6 @@
     <t>05 Envoyer des données à l’IHM OK</t>
   </si>
   <si>
-    <t>06 Navigation interne OK</t>
-  </si>
-  <si>
     <t>07 Navigation externe</t>
   </si>
   <si>
@@ -483,6 +480,18 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>06 Navigation interne KO</t>
+  </si>
+  <si>
+    <t>11 Tester L'application</t>
+  </si>
+  <si>
+    <t>Junit</t>
+  </si>
+  <si>
+    <t>Expresso</t>
   </si>
 </sst>
 </file>
@@ -876,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,64 +902,60 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8">
-        <f>SUM(A2:A88)</f>
-        <v>175381</v>
+        <f>SUM(A2:A91)</f>
+        <v>274381</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
         <v>147</v>
-      </c>
-      <c r="D1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12000</v>
       </c>
-      <c r="B2">
-        <f>SUM(A2)</f>
-        <v>12000</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" t="s">
         <v>126</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>127</v>
-      </c>
-      <c r="H3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2">
@@ -968,147 +973,139 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
         <v>129</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>130</v>
-      </c>
-      <c r="H5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" t="s">
         <v>132</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>133</v>
-      </c>
-      <c r="H6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" t="s">
         <v>135</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>136</v>
-      </c>
-      <c r="H7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>26000</v>
       </c>
-      <c r="B8">
-        <f>SUM(A2:A8)/2</f>
-        <v>19000</v>
-      </c>
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" t="s">
         <v>138</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>139</v>
-      </c>
-      <c r="H9" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" t="s">
         <v>141</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>142</v>
-      </c>
-      <c r="H10" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
         <v>26</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>45749</v>
       </c>
-      <c r="B14">
-        <f>SUM(A2:A14)/3</f>
-        <v>27916.333333333332</v>
-      </c>
       <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1116,57 +1113,53 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>64187</v>
       </c>
-      <c r="B20">
-        <f>SUM(A2:A20)/4</f>
-        <v>36984</v>
-      </c>
       <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
@@ -1174,76 +1167,72 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27445</v>
       </c>
-      <c r="B26">
-        <f>SUM(A2:A26)/5</f>
-        <v>35076.199999999997</v>
-      </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2" t="b">
@@ -1252,7 +1241,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="b">
@@ -1261,420 +1250,468 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>13000</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10000</v>
+      </c>
       <c r="C38" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>15000</v>
+      </c>
       <c r="C44" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" t="s">
         <v>64</v>
       </c>
-      <c r="F47" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>15000</v>
+      </c>
       <c r="C50" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="1" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C54" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="1" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10000</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>17000</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="1" t="s">
+      <c r="D60" s="1"/>
+      <c r="E60" t="s">
         <v>80</v>
       </c>
-      <c r="D57" s="1"/>
-      <c r="E57" t="s">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C61" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C58" s="1" t="s">
+      <c r="D61" s="1"/>
+      <c r="E61" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="2" t="s">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C62" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" s="1" t="s">
+      <c r="D62" s="1"/>
+      <c r="E62" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="2" t="s">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C63" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D60" s="1"/>
-      <c r="E60" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C62" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C63" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D64" s="1"/>
-      <c r="E64" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>10000</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C67" s="1" t="s">
+      <c r="D70" s="1"/>
+      <c r="E70" t="s">
         <v>97</v>
       </c>
-      <c r="D67" s="1"/>
-      <c r="E67" t="s">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>4000</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C68" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" s="4"/>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C69" s="1" t="s">
+      <c r="D72" s="1"/>
+      <c r="E72" t="s">
         <v>99</v>
       </c>
-      <c r="D69" s="1"/>
-      <c r="E69" t="s">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C73" s="1" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C70" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C71" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C72" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C73" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C74" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>5000</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C78" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C79" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C76" s="1" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C80" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C77" s="1" t="s">
+      <c r="D80" s="1"/>
+      <c r="E80" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>115</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="2" t="b">
+      <c r="E81" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E78" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C79" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D79" s="1"/>
-      <c r="E79" s="2" t="b">
+      <c r="D82" s="1"/>
+      <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mis a jour du mardi
</commit_message>
<xml_diff>
--- a/Nouveau livre/Quizz.xlsx
+++ b/Nouveau livre/Quizz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kotlin_be_back\Kotlin_be_back\Nouveau livre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kotlin_be_back\Nouveau livre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A58CEE-AAAC-4E90-BDCA-633D8D152DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B42B08-3AA6-4353-BA21-76E773C302FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="154">
   <si>
     <t>01 Présentation de l’environnement OK</t>
   </si>
@@ -59,9 +59,6 @@
     <t>09 ViewModel et LiveData OK</t>
   </si>
   <si>
-    <t>13 Firebase</t>
-  </si>
-  <si>
     <t>L'architecture Android est basée sur :</t>
   </si>
   <si>
@@ -464,15 +461,6 @@
     <t>JavaScript</t>
   </si>
   <si>
-    <t>10 L’ORM Room OK</t>
-  </si>
-  <si>
-    <t>11 RecyclerView OK</t>
-  </si>
-  <si>
-    <t>12 Communiquer avec une API REST OK</t>
-  </si>
-  <si>
     <t>Taux</t>
   </si>
   <si>
@@ -485,13 +473,28 @@
     <t>06 Navigation interne KO</t>
   </si>
   <si>
-    <t>11 Tester L'application</t>
-  </si>
-  <si>
     <t>Junit</t>
   </si>
   <si>
     <t>Expresso</t>
+  </si>
+  <si>
+    <t>10 Tester L'application</t>
+  </si>
+  <si>
+    <t>11 L’ORM Room OK</t>
+  </si>
+  <si>
+    <t>12 RecyclerView OK</t>
+  </si>
+  <si>
+    <t>13 Communiquer avec une API REST OK</t>
+  </si>
+  <si>
+    <t>14 Firebase</t>
+  </si>
+  <si>
+    <t>15 Les éléments avancés</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -600,6 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,13 +908,13 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8">
         <f>SUM(A2:A91)</f>
-        <v>274381</v>
+        <v>369381</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,42 +925,42 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
         <v>125</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>126</v>
-      </c>
-      <c r="H3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2">
@@ -974,56 +978,56 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" t="s">
         <v>128</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>129</v>
-      </c>
-      <c r="H5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" t="s">
         <v>131</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>132</v>
-      </c>
-      <c r="H6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" t="s">
         <v>134</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>135</v>
-      </c>
-      <c r="H7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1034,73 +1038,73 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" t="s">
         <v>137</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>138</v>
-      </c>
-      <c r="H9" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G10" t="s">
         <v>140</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>141</v>
-      </c>
-      <c r="H10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
         <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1114,47 +1118,47 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,38 +1172,38 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1210,30 +1214,30 @@
         <v>4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2" t="b">
@@ -1242,7 +1246,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="b">
@@ -1251,63 +1255,63 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>13000</v>
+        <v>14000</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="2" t="b">
@@ -1325,34 +1329,34 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="2" t="b">
@@ -1361,11 +1365,11 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,7 +1383,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="2" t="b">
@@ -1388,41 +1392,41 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" t="s">
         <v>63</v>
-      </c>
-      <c r="F47" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,47 +1440,47 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,20 +1488,20 @@
         <v>10000</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D58" s="1"/>
     </row>
@@ -1506,49 +1510,49 @@
         <v>17000</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C60" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C62" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="2" t="b">
@@ -1560,161 +1564,170 @@
         <v>10000</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>4000</v>
+        <v>12000</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C76" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>5000</v>
+        <v>11000</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="D77" s="4"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C78" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C79" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C80" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E81" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C82" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>80000</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D83" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>